<commit_message>
fix some bugs and change searching url to google.com
</commit_message>
<xml_diff>
--- a/result/Mother+Courage.xlsx
+++ b/result/Mother+Courage.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
-  <si>
-    <t>117,000,000</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="71">
+  <si>
+    <t>147,000,000</t>
   </si>
   <si>
     <t>title</t>
@@ -49,24 +49,78 @@
     <t>https://www.sparknotes.com/drama/mothercourage/summary/</t>
   </si>
   <si>
-    <t>Mother Courage and Her Children: Study Guide - SparkNotes</t>
-  </si>
-  <si>
-    <t>Mother Courage and Her Children is a play by Bertolt Brecht that was first performed in 1941. Summary. Read one-minute Sparklet summaries, the detailed scene-by ...</t>
-  </si>
-  <si>
-    <t>https://www.sparknotes.com/drama/mothercourage/</t>
-  </si>
-  <si>
     <t>Mother Courage and Her Children | play by Brecht | Britannica</t>
   </si>
   <si>
-    <t>The plot revolves around a woman who depends on war for her personal survival and who is nicknamed Mother Courage for her coolness in safeguarding her ...</t>
+    <t>The work, composed of 12 scenes, is a chronicle play of the Thirty Years' War and is based on the picaresque novel Simplicissimus (1669) by Hans Jacob Christoph ...</t>
   </si>
   <si>
     <t>https://www.britannica.com/topic/Mother-Courage-and-Her-Children</t>
   </si>
   <si>
+    <t>Mother Courage and Her Children: Bertolt Brecht, Eric Bentley</t>
+  </si>
+  <si>
+    <t>Set in the seventeenth century, the play follows Anna Fierling (“Mother Courage”), an itinerant trader, as she pulls her wagon of wares and her children through ...</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Mother-Courage-Children-Bertolt-Brecht/dp/0802130828</t>
+  </si>
+  <si>
+    <t>Production History | Mother Courage and Her Children</t>
+  </si>
+  <si>
+    <t>by B Brecht — There are two productions of Brecht's Mother Courage and Her Children (Mutter Courage und ihre Kinder) that are frequently considered the “original” ...</t>
+  </si>
+  <si>
+    <t>https://journeys.dartmouth.edu/mothercourage/production-history/</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children Summary | GradeSaver</t>
+  </si>
+  <si>
+    <t>Dec 14, 2022 — The play is set in Europe during the Thirty Years' War. Mother Courage, a canteen woman, pulls her cart with her three children (Eilif, ...</t>
+  </si>
+  <si>
+    <t>https://www.gradesaver.com/mother-courage-and-her-children/study-guide/summary</t>
+  </si>
+  <si>
+    <t>'Mother Courage' Review: Selling Her Wares Amid the Havoc ...</t>
+  </si>
+  <si>
+    <t>May 25, 2022 — Mother Courage (an appropriately brusque Vicky Gilmore, in a knit hat, leather jacket and combat boots), traveling with her three children, is ...</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2022/05/25/theater/mother-courage-and-her-children-review.html</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children | Theater in New York</t>
+  </si>
+  <si>
+    <t>Aug 18, 2006 — Mother Courage and Her Children: Review by Adam FeldmanTo her great credit, Meryl Streep seems genuinely exhausted by the end of Mother ...</t>
+  </si>
+  <si>
+    <t>https://www.timeout.com/newyork/theater/mother-courage-and-her-children-2</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children Summary - SuperSummary</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children (1939) is the antiwar musical stage-play written by exiled German dramatist Bertolt Brecht. Set in seventeenth-century ...</t>
+  </si>
+  <si>
+    <t>https://www.supersummary.com/mother-courage-and-her-children/summary/</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children - Classic Stage Company</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children. January 1-31, 2016. BY BERTOLT BRECHT DIRECTED BY BRIAN KULICK. CSC continues its exploration of Bertolt Brecht with a look ...</t>
+  </si>
+  <si>
+    <t>https://www.classicstage.org/show-archive/mother-courage</t>
+  </si>
+  <si>
     <t>Mother Courage and Her Children | DEFA Film Library</t>
   </si>
   <si>
@@ -76,13 +130,76 @@
     <t>https://www.umass.edu/defa/film/37964</t>
   </si>
   <si>
-    <t>Mother Courage and Her Children - Amazon.com</t>
-  </si>
-  <si>
-    <t>Mother Courage and Her Children [Bertolt Brecht, Eric Bentley] on Amazon.com. *FREE* shipping on qualifying offers. Mother Courage and Her Children.</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Mother-Courage-Children-Bertolt-Brecht/dp/0802130828</t>
+    <t>Mother Courage and Her Children Introduction | Shmoop</t>
+  </si>
+  <si>
+    <t>Written in Sweden in 1939 at the height of World War II by exiled German playwright Bertolt Brecht, Mother Courage has an important thing or two to say ...</t>
+  </si>
+  <si>
+    <t>https://www.shmoop.com/study-guides/literature/mother-courage-and-her-children</t>
+  </si>
+  <si>
+    <t>Theatre / Mother Courage and Her Children - TV Tropes</t>
+  </si>
+  <si>
+    <t>A description of tropes appearing in Mother Courage and Her Children. 1624. The Protestant King of Sweden has invaded Catholic Poland. Mainland Europe, …</t>
+  </si>
+  <si>
+    <t>https://tvtropes.org/pmwiki/pmwiki.php/Theatre/MotherCourageAndHerChildren</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children (Bentley, trans.)</t>
+  </si>
+  <si>
+    <t>This German play was written in 1939 and was first produced in Zurich in 1941. In America, it was published in English right away (1941, by New Directions) but ...</t>
+  </si>
+  <si>
+    <t>https://www.concordtheatricals.com/p/996/mother-courage-and-her-children-bentley-trans</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children. (1939) by Bertolt Brecht. Digitalized by. RevSocialist for. SocialistStories. Page 2. Page 3. Page 4. Page 5. Page 6 ...</t>
+  </si>
+  <si>
+    <t>https://edisciplinas.usp.br/mod/resource/view.php?id=2217102</t>
+  </si>
+  <si>
+    <t>The Meryl Streep Archives » Mother Courage and Her Children</t>
+  </si>
+  <si>
+    <t>As Mother Courage seeks to profit from the war that is killing her children, she questions the roles of honesty, virtue and family in the face of a bitter ...</t>
+  </si>
+  <si>
+    <t>http://www.simplystreep.com/projects/2006-mother-courage-and-her-children/</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children | Encyclopedia.com</t>
+  </si>
+  <si>
+    <t>First produced in Zurich, Switzerland, in 1939, Bertolt Brecht's Mother Courage and Her Children is considered by many to be among the playwright's best ...</t>
+  </si>
+  <si>
+    <t>https://www.encyclopedia.com/arts/educational-magazines/mother-courage-and-her-children</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children by Bertolt Brecht ... - Events</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children by Bertolt Brecht, Translated by Eric Bentley. Thursday, September 29, 2022 , 7:30 pm – 10:00 pm.</t>
+  </si>
+  <si>
+    <t>https://events.illinoisstate.edu/event/mother-courage-and-her-children-by-bertolt-brecht-translated-by-eric-bentley/2022-09-29/</t>
+  </si>
+  <si>
+    <t>Bluff Your Way Through the Play: Mother Courage and Her ...</t>
+  </si>
+  <si>
+    <t>How'd She Get the Name? Mother Courage was a nickname given to business woman Anna Fierling when she ran through a battle in order to sell loaves of bread ...</t>
+  </si>
+  <si>
+    <t>https://www.seattleshakespeare.org/bluff-mother-courage/</t>
   </si>
   <si>
     <t>Mother Courage and Her Children (Play) Plot &amp; Characters</t>
@@ -94,13 +211,22 @@
     <t>https://stageagent.com/shows/play/3628/mother-courage-and-her-children</t>
   </si>
   <si>
-    <t>Mother Courage and Her Children - Classic Stage Company</t>
-  </si>
-  <si>
-    <t>CSC continues its exploration of Bertolt Brecht with a look at his most famous play. The indomitable Mother Courage follows one luckless army after another ...</t>
-  </si>
-  <si>
-    <t>https://www.classicstage.org/show-archive/mother-courage</t>
+    <t>Book review -- By Bertolt Brecht – MOTHER COURAGE</t>
+  </si>
+  <si>
+    <t>Mother Courage sees life as a struggle to survive and get by. She can't control the larger forces so she works out how to survive for herself and children, at ...</t>
+  </si>
+  <si>
+    <t>http://faculty.webster.edu/corbetre/personal/reading/brecht-courage.html</t>
+  </si>
+  <si>
+    <t>Mother Courage and Her Children - FringeArts</t>
+  </si>
+  <si>
+    <t>September 13, 15, 18 + 21, 2019. Mother Courage drags her cart across the battlefields of the Thirty Years War, profiteering from a conflict that destroys ...</t>
+  </si>
+  <si>
+    <t>https://fringearts.com/event/mother-courage-and-her-children/</t>
   </si>
 </sst>
 </file>
@@ -445,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,13 +694,517 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -587,6 +1217,42 @@
     <hyperlink ref="D7" r:id="rId6"/>
     <hyperlink ref="D8" r:id="rId7"/>
     <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>